<commit_message>
Recorded data for OH226W48H
</commit_message>
<xml_diff>
--- a/Corina's Data Spreadsheet.xlsx
+++ b/Corina's Data Spreadsheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdnewsome1\Documents\THESIS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdnewsome1\Documents\GitHub\Beetle-Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="205">
   <si>
     <t>Population</t>
   </si>
@@ -635,6 +635,12 @@
   </si>
   <si>
     <t>DEFGJ48HC2</t>
+  </si>
+  <si>
+    <t>asdfl</t>
+  </si>
+  <si>
+    <t>sadf</t>
   </si>
 </sst>
 </file>
@@ -4698,8 +4704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DW56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N32" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="R54" sqref="R54"/>
+    <sheetView tabSelected="1" topLeftCell="DK1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="DU1" sqref="DU1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5444,6 +5450,9 @@
       <c r="DT2" t="s">
         <v>74</v>
       </c>
+      <c r="DU2" t="s">
+        <v>203</v>
+      </c>
       <c r="DV2" t="s">
         <v>170</v>
       </c>
@@ -5607,6 +5616,9 @@
       </c>
       <c r="DS3">
         <v>3024</v>
+      </c>
+      <c r="DU3" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:127" x14ac:dyDescent="0.25">

</xml_diff>